<commit_message>
Poprawki na podstawie retrospektywi Sprintu 1
Dodanie nieukończonego punktu z pierwszego sprintu, 
Dodanie punktu o poprawie kompozytu.
</commit_message>
<xml_diff>
--- a/Sprint Backlog 2.xlsx
+++ b/Sprint Backlog 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\przem\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Łukasz Frątczak\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04460DF7-A147-402E-8ECD-2818A9D499BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E747ED38-824B-4A5E-8C14-2AA685F9ED08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog #1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Element rejestru produktu</t>
   </si>
@@ -83,6 +83,27 @@
   </si>
   <si>
     <t>Dodanie funkcjonalności, która pozwala zamknąć komunikat po potwierdzeniu przez zarządcę budynku</t>
+  </si>
+  <si>
+    <t>Jako zarządca budynku mogę otrzymać informację o pomieszczeniach w budynku, które przekraczają określony poziom zużycia energii cieplnej / m^3 podany jako parametr, aby znaleźć miejsca do poprawy w infrastrukturze.</t>
+  </si>
+  <si>
+    <t>Zaimplementowanie poszukiwania pomieszczeń przekraczającyh określony poziom zużycia energi cieplnej</t>
+  </si>
+  <si>
+    <t>Pobieranie podanej przez administratora wartości energii</t>
+  </si>
+  <si>
+    <t>Wyświetlenie znalezionych pomieszczeń</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Poprawienie wzorca kopmpozyt</t>
+  </si>
+  <si>
+    <t>Poprawienie funkcji tak aby operowały na abstrakcji</t>
   </si>
 </sst>
 </file>
@@ -233,6 +254,15 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -251,15 +281,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -274,12 +295,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A4:C44" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A4:C44" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A4:C44" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Element rejestru produktu" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Zadania" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Pracochłonność " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Element rejestru produktu" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Zadania" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Pracochłonność " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -735,7 +756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -743,12 +764,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>